<commit_message>
fix: Reset failedRows array after billing process completion
</commit_message>
<xml_diff>
--- a/public/plantilla_facturacion.xlsx
+++ b/public/plantilla_facturacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ufred\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B820CF53-A80B-456D-849D-DD530BC9453C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B323ED-3365-4F1B-84C7-22A65E2D197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{92A98749-9D5D-4931-84C4-6886474B4307}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Código</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Precio</t>
-  </si>
-  <si>
-    <t>Método de pago</t>
   </si>
 </sst>
 </file>
@@ -434,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37161C2B-FACA-408E-9EC6-A1A065E78A4D}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,9 +463,6 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>